<commit_message>
runmodes added- excel sheet
</commit_message>
<xml_diff>
--- a/BankProject1/src/test/resources/excel/testdata.xlsx
+++ b/BankProject1/src/test/resources/excel/testdata.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\automation\LocalRepoGit\BankProject1LR2\BankProject1\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E63209-3BFB-4DD2-AF75-E51D4414CAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB0EE08-1374-47F3-80A4-D9FB2EA80C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12300" yWindow="756" windowWidth="8388" windowHeight="7584" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="1" sheetId="4" r:id="rId2"/>
     <sheet name="TC2addCustomer" sheetId="1" r:id="rId3"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId4"/>
+    <sheet name="TC3OpenAccount" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>firstname</t>
   </si>
@@ -39,15 +39,6 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>A234wd</t>
-  </si>
-  <si>
     <t>alerttext</t>
   </si>
   <si>
@@ -60,46 +51,97 @@
     <t>currency</t>
   </si>
   <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
     <t>Rupee</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
     <t>Runmode</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>runmode</t>
+  </si>
+  <si>
+    <t>anish</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>dfdsf</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>fgfg</t>
+  </si>
+  <si>
+    <t>Nita</t>
+  </si>
+  <si>
+    <t>Kulkarni</t>
+  </si>
+  <si>
+    <t>ghgf</t>
+  </si>
+  <si>
+    <t>Rajiv</t>
+  </si>
+  <si>
+    <t>Parv</t>
+  </si>
+  <si>
+    <t>hgg</t>
+  </si>
+  <si>
+    <t>Ganga</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>hjh</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Sankar</t>
+  </si>
+  <si>
+    <t>mhjk</t>
+  </si>
+  <si>
+    <t>Anita Jacob</t>
+  </si>
+  <si>
+    <t>TC1BankManagerLogin</t>
+  </si>
+  <si>
+    <t>TC3OpenAccount</t>
+  </si>
+  <si>
+    <t>asas546</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>tester1</t>
+  </si>
+  <si>
+    <t>TC2AddCustomer</t>
   </si>
 </sst>
 </file>
@@ -420,41 +462,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +512,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,21 +531,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -510,10 +555,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,78 +577,106 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -615,26 +688,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>